<commit_message>
Tests update (parametrization added), Database check implemented
</commit_message>
<xml_diff>
--- a/users_creator/users.xlsx
+++ b/users_creator/users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kirill\3_Work\EPM-AGL\AGLS_AT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kirill\3_Work\EPM-AGL\AGLS_AT\users_creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E32F553-83B6-4C24-B19D-93FDCBCAAEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16541A53-1FC0-4446-A61F-51001EC44CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="3360" windowWidth="15660" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>email</t>
   </si>
@@ -36,22 +36,31 @@
     <t>last_name</t>
   </si>
   <si>
-    <t>Kirill</t>
-  </si>
-  <si>
-    <t>Khr</t>
-  </si>
-  <si>
-    <t>kirill@mail.de</t>
-  </si>
-  <si>
-    <t>Tonya</t>
-  </si>
-  <si>
-    <t>Sh</t>
-  </si>
-  <si>
-    <t>tonya@mail.fr</t>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>first_member@mail.com</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>second_member@mail.com</t>
+  </si>
+  <si>
+    <t>third_member@mail.com</t>
+  </si>
+  <si>
+    <t>fourth_member@mail.com</t>
   </si>
 </sst>
 </file>
@@ -421,17 +430,33 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
@@ -443,6 +468,8 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{755D7AFD-88D6-4009-A9EA-9FBA0B816D0D}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{7613D26B-8FC9-46F4-9533-0FB462FE2BF1}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{047BFD76-116F-4C4E-A35E-6DBC4F0CFCE7}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{D6C770A4-CF14-4747-AAB7-94F474059BEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New methods were added, Quick access page test suite was created
</commit_message>
<xml_diff>
--- a/users_creator/users.xlsx
+++ b/users_creator/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kirill\3_Work\EPM-AGL\AGLS_AT\users_creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB73D54-C52E-479E-8309-16CAE5557576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20045DF-52CE-4B47-B8A8-97A856B17B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +79,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF343541"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,9 +109,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -386,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,9 +406,10 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -414,7 +423,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -428,7 +437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -442,7 +451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -455,6 +464,9 @@
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="15" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="E15" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -463,5 +475,6 @@
     <hyperlink ref="D4" r:id="rId3" xr:uid="{7EFE4C04-92A6-424D-A253-562AF9BDC271}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Database connection was adjusted, "feedback" modal tests were added with db check
</commit_message>
<xml_diff>
--- a/users_creator/users.xlsx
+++ b/users_creator/users.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kirill\3_Work\EPM-AGL\AGLS_AT\users_creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20045DF-52CE-4B47-B8A8-97A856B17B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A01F022E-3099-4957-ACB1-5C1176130739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{FE166C93-95C7-4336-A272-BD8A3A445F44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -27,6 +36,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
+    <t>idn</t>
+  </si>
+  <si>
     <t>first_name</t>
   </si>
   <si>
@@ -39,32 +51,29 @@
     <t>First</t>
   </si>
   <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>first_member@mail.com</t>
+  </si>
+  <si>
     <t>Second</t>
   </si>
   <si>
+    <t>second_member@mail.com</t>
+  </si>
+  <si>
     <t>Third</t>
   </si>
   <si>
-    <t>Member</t>
-  </si>
-  <si>
-    <t>first_member@mail.com</t>
-  </si>
-  <si>
-    <t>second_member@mail.com</t>
-  </si>
-  <si>
     <t>third_member@mail.com</t>
-  </si>
-  <si>
-    <t>idn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,13 +88,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF343541"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,10 +111,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -148,7 +149,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -160,7 +161,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -207,6 +208,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -242,6 +260,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -393,11 +428,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A292CBD-91C6-49F0-8BDF-018B640B664C}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,75 +441,70 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="E15" s="2"/>
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{04D41025-F580-497D-85C4-D71763C979F6}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{14F29C16-DAB3-4AA9-A302-3379F22FBA4F}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{7EFE4C04-92A6-424D-A253-562AF9BDC271}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{DC113F23-2152-4757-9541-0D8C2A039159}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{D5DE3CA3-BDDA-492F-B664-C50D9D6C7184}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{A087D7F5-3551-4D79-A934-0632EB83FF92}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sign Up page tests were added
</commit_message>
<xml_diff>
--- a/users_creator/users.xlsx
+++ b/users_creator/users.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Kirill\3_Work\EPM-AGL\AGLS_AT\users_creator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A01F022E-3099-4957-ACB1-5C1176130739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8394FB-9215-4B97-8381-1BD5344EF2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{FE166C93-95C7-4336-A272-BD8A3A445F44}"/>
+    <workbookView xWindow="2145" yWindow="3165" windowWidth="15660" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -73,18 +64,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,16 +90,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -149,7 +129,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -161,7 +141,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -208,23 +188,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -260,23 +223,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -428,11 +374,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A292CBD-91C6-49F0-8BDF-018B640B664C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +413,7 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -481,7 +427,7 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -495,16 +441,11 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{DC113F23-2152-4757-9541-0D8C2A039159}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{D5DE3CA3-BDDA-492F-B664-C50D9D6C7184}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{A087D7F5-3551-4D79-A934-0632EB83FF92}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>